<commit_message>
Add Objetivo e Justificativa do Projeto
</commit_message>
<xml_diff>
--- a/docs/backlog_HelpEnterprising.xlsx
+++ b/docs/backlog_HelpEnterprising.xlsx
@@ -3,17 +3,21 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Burndown - Sprint 1" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Burndown - Sprint 2" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Burndown - Sprint 3" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Burndown - Sprint 4" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t xml:space="preserve">Backlog do Projeto</t>
   </si>
@@ -37,13 +41,49 @@
   </si>
   <si>
     <t>Outros</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Burndown SPRINT 01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dia 01 (3 Pontos)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dia 02 (6 Pontos)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dia 03 (12 Pontos)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dia 04 (15 Pontos)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Burndown SPRINT 02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dia 01 (X Pontos)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dia 02 (X Pontos)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dia 03 (X Pontos)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dia 04 (X Pontos)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Burndown SPRINT 03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Burndown SPRINT 04</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <name val="Calibri"/>
       <color theme="1"/>
@@ -99,6 +139,19 @@
       <sz val="11.000000"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <b/>
+      <color theme="1"/>
+      <sz val="18.000000"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <color theme="1"/>
+      <sz val="16.000000"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -120,7 +173,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -173,11 +226,40 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="19">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -214,6 +296,18 @@
     </xf>
     <xf fontId="7" fillId="3" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="8" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="4" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="5" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="6" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="9" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="9" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -967,4 +1061,540 @@
   <headerFooter/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0" zoomScale="100">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col customWidth="1" min="3" max="3" width="14.421875"/>
+    <col customWidth="1" min="7" max="7" width="14.8515625"/>
+    <col customWidth="1" min="11" max="11" width="17.28125"/>
+    <col customWidth="1" min="14" max="14" width="16.28125"/>
+  </cols>
+  <sheetData>
+    <row r="2" ht="23.25">
+      <c r="F2" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+    </row>
+    <row r="6" ht="14.25">
+      <c r="B6" s="14"/>
+    </row>
+    <row r="7" ht="14.25">
+      <c r="B7" s="14"/>
+    </row>
+    <row r="8" ht="14.25">
+      <c r="B8" s="14"/>
+    </row>
+    <row r="9" ht="14.25">
+      <c r="B9" s="14"/>
+    </row>
+    <row r="10" ht="14.25">
+      <c r="B10" s="14"/>
+    </row>
+    <row r="11" ht="14.25">
+      <c r="B11" s="14"/>
+    </row>
+    <row r="12" ht="14.25">
+      <c r="B12" s="14"/>
+    </row>
+    <row r="13" ht="14.25">
+      <c r="B13" s="14"/>
+    </row>
+    <row r="14" ht="14.25">
+      <c r="B14" s="14"/>
+    </row>
+    <row r="15" ht="14.25">
+      <c r="B15" s="14"/>
+    </row>
+    <row r="16" ht="14.25">
+      <c r="B16" s="14"/>
+    </row>
+    <row r="17" ht="14.25">
+      <c r="B17" s="14"/>
+    </row>
+    <row r="18" ht="14.25">
+      <c r="B18" s="14"/>
+    </row>
+    <row r="19" ht="14.25">
+      <c r="B19" s="14"/>
+    </row>
+    <row r="20" ht="14.25">
+      <c r="B20" s="14"/>
+    </row>
+    <row r="21" ht="14.25">
+      <c r="B21" s="14"/>
+    </row>
+    <row r="22" ht="14.25">
+      <c r="B22" s="14"/>
+    </row>
+    <row r="23" ht="14.25">
+      <c r="B23" s="14"/>
+    </row>
+    <row r="24" ht="14.25">
+      <c r="B24" s="14"/>
+    </row>
+    <row r="25" ht="14.25">
+      <c r="B25" s="14"/>
+    </row>
+    <row r="26" ht="14.25">
+      <c r="B26" s="14"/>
+    </row>
+    <row r="27" ht="14.25">
+      <c r="B27" s="15"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="16"/>
+      <c r="I27" s="16"/>
+      <c r="J27" s="16"/>
+      <c r="K27" s="16"/>
+      <c r="L27" s="16"/>
+      <c r="M27" s="16"/>
+      <c r="N27" s="16"/>
+    </row>
+    <row r="28" ht="21">
+      <c r="B28" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="17"/>
+      <c r="F28" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G28" s="18"/>
+      <c r="J28" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="K28" s="18"/>
+      <c r="M28" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="N28" s="18"/>
+    </row>
+    <row r="31" ht="14.25"/>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="M28:N28"/>
+  </mergeCells>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup blackAndWhite="0" cellComments="none" copies="1" draft="0" errors="displayed" firstPageNumber="-1" fitToHeight="1" fitToWidth="1" horizontalDpi="600" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" usePrinterDefaults="1" verticalDpi="600"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0" zoomScale="100">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col customWidth="1" min="3" max="3" width="14.421875"/>
+    <col customWidth="1" min="7" max="7" width="14.8515625"/>
+    <col customWidth="1" min="11" max="11" width="17.28125"/>
+    <col customWidth="1" min="14" max="14" width="16.28125"/>
+  </cols>
+  <sheetData>
+    <row r="2" ht="23.25">
+      <c r="F2" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+    </row>
+    <row r="6" ht="14.25">
+      <c r="B6" s="14"/>
+    </row>
+    <row r="7" ht="14.25">
+      <c r="B7" s="14"/>
+    </row>
+    <row r="8" ht="14.25">
+      <c r="B8" s="14"/>
+    </row>
+    <row r="9" ht="14.25">
+      <c r="B9" s="14"/>
+    </row>
+    <row r="10" ht="14.25">
+      <c r="B10" s="14"/>
+    </row>
+    <row r="11" ht="14.25">
+      <c r="B11" s="14"/>
+    </row>
+    <row r="12" ht="14.25">
+      <c r="B12" s="14"/>
+    </row>
+    <row r="13" ht="14.25">
+      <c r="B13" s="14"/>
+    </row>
+    <row r="14" ht="14.25">
+      <c r="B14" s="14"/>
+    </row>
+    <row r="15" ht="14.25">
+      <c r="B15" s="14"/>
+    </row>
+    <row r="16" ht="14.25">
+      <c r="B16" s="14"/>
+    </row>
+    <row r="17" ht="14.25">
+      <c r="B17" s="14"/>
+    </row>
+    <row r="18" ht="14.25">
+      <c r="B18" s="14"/>
+    </row>
+    <row r="19" ht="14.25">
+      <c r="B19" s="14"/>
+    </row>
+    <row r="20" ht="14.25">
+      <c r="B20" s="14"/>
+    </row>
+    <row r="21" ht="14.25">
+      <c r="B21" s="14"/>
+    </row>
+    <row r="22" ht="14.25">
+      <c r="B22" s="14"/>
+    </row>
+    <row r="23" ht="14.25">
+      <c r="B23" s="14"/>
+    </row>
+    <row r="24" ht="14.25">
+      <c r="B24" s="14"/>
+    </row>
+    <row r="25" ht="14.25">
+      <c r="B25" s="14"/>
+    </row>
+    <row r="26" ht="14.25">
+      <c r="B26" s="14"/>
+    </row>
+    <row r="27" ht="14.25">
+      <c r="B27" s="15"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="16"/>
+      <c r="I27" s="16"/>
+      <c r="J27" s="16"/>
+      <c r="K27" s="16"/>
+      <c r="L27" s="16"/>
+      <c r="M27" s="16"/>
+      <c r="N27" s="16"/>
+    </row>
+    <row r="28" ht="21">
+      <c r="B28" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C28" s="17"/>
+      <c r="F28" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="G28" s="18"/>
+      <c r="J28" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="K28" s="18"/>
+      <c r="M28" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="N28" s="18"/>
+    </row>
+    <row r="31" ht="14.25"/>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="M28:N28"/>
+  </mergeCells>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup blackAndWhite="0" cellComments="none" copies="1" draft="0" errors="displayed" firstPageNumber="-1" fitToHeight="1" fitToWidth="1" horizontalDpi="600" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" usePrinterDefaults="1" verticalDpi="600"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0" zoomScale="100">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col customWidth="1" min="3" max="3" width="14.421875"/>
+    <col customWidth="1" min="7" max="7" width="14.8515625"/>
+    <col customWidth="1" min="11" max="11" width="17.28125"/>
+    <col customWidth="1" min="14" max="14" width="16.28125"/>
+  </cols>
+  <sheetData>
+    <row r="2" ht="23.25">
+      <c r="F2" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+    </row>
+    <row r="6" ht="14.25">
+      <c r="B6" s="14"/>
+    </row>
+    <row r="7" ht="14.25">
+      <c r="B7" s="14"/>
+    </row>
+    <row r="8" ht="14.25">
+      <c r="B8" s="14"/>
+    </row>
+    <row r="9" ht="14.25">
+      <c r="B9" s="14"/>
+    </row>
+    <row r="10" ht="14.25">
+      <c r="B10" s="14"/>
+    </row>
+    <row r="11" ht="14.25">
+      <c r="B11" s="14"/>
+    </row>
+    <row r="12" ht="14.25">
+      <c r="B12" s="14"/>
+    </row>
+    <row r="13" ht="14.25">
+      <c r="B13" s="14"/>
+    </row>
+    <row r="14" ht="14.25">
+      <c r="B14" s="14"/>
+    </row>
+    <row r="15" ht="14.25">
+      <c r="B15" s="14"/>
+    </row>
+    <row r="16" ht="14.25">
+      <c r="B16" s="14"/>
+    </row>
+    <row r="17" ht="14.25">
+      <c r="B17" s="14"/>
+    </row>
+    <row r="18" ht="14.25">
+      <c r="B18" s="14"/>
+    </row>
+    <row r="19" ht="14.25">
+      <c r="B19" s="14"/>
+    </row>
+    <row r="20" ht="14.25">
+      <c r="B20" s="14"/>
+    </row>
+    <row r="21" ht="14.25">
+      <c r="B21" s="14"/>
+    </row>
+    <row r="22" ht="14.25">
+      <c r="B22" s="14"/>
+    </row>
+    <row r="23" ht="14.25">
+      <c r="B23" s="14"/>
+    </row>
+    <row r="24" ht="14.25">
+      <c r="B24" s="14"/>
+    </row>
+    <row r="25" ht="14.25">
+      <c r="B25" s="14"/>
+    </row>
+    <row r="26" ht="14.25">
+      <c r="B26" s="14"/>
+    </row>
+    <row r="27" ht="14.25">
+      <c r="B27" s="15"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="16"/>
+      <c r="I27" s="16"/>
+      <c r="J27" s="16"/>
+      <c r="K27" s="16"/>
+      <c r="L27" s="16"/>
+      <c r="M27" s="16"/>
+      <c r="N27" s="16"/>
+    </row>
+    <row r="28" ht="21">
+      <c r="B28" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C28" s="17"/>
+      <c r="F28" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="G28" s="18"/>
+      <c r="K28" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="L28" s="17"/>
+      <c r="M28" s="18"/>
+      <c r="N28" s="18"/>
+    </row>
+    <row r="31" ht="14.25"/>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="M28:N28"/>
+  </mergeCells>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup blackAndWhite="0" cellComments="none" copies="1" draft="0" errors="displayed" firstPageNumber="-1" fitToHeight="1" fitToWidth="1" horizontalDpi="600" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" usePrinterDefaults="1" verticalDpi="600"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0" zoomScale="100">
+      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col customWidth="1" min="3" max="3" width="14.421875"/>
+    <col customWidth="1" min="7" max="7" width="14.8515625"/>
+    <col customWidth="1" min="11" max="11" width="17.28125"/>
+    <col customWidth="1" min="14" max="14" width="16.28125"/>
+  </cols>
+  <sheetData>
+    <row r="2" ht="23.25">
+      <c r="F2" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+    </row>
+    <row r="6" ht="14.25">
+      <c r="B6" s="14"/>
+    </row>
+    <row r="7" ht="14.25">
+      <c r="B7" s="14"/>
+    </row>
+    <row r="8" ht="14.25">
+      <c r="B8" s="14"/>
+    </row>
+    <row r="9" ht="14.25">
+      <c r="B9" s="14"/>
+    </row>
+    <row r="10" ht="14.25">
+      <c r="B10" s="14"/>
+    </row>
+    <row r="11" ht="14.25">
+      <c r="B11" s="14"/>
+    </row>
+    <row r="12" ht="14.25">
+      <c r="B12" s="14"/>
+    </row>
+    <row r="13" ht="14.25">
+      <c r="B13" s="14"/>
+    </row>
+    <row r="14" ht="14.25">
+      <c r="B14" s="14"/>
+    </row>
+    <row r="15" ht="14.25">
+      <c r="B15" s="14"/>
+    </row>
+    <row r="16" ht="14.25">
+      <c r="B16" s="14"/>
+    </row>
+    <row r="17" ht="14.25">
+      <c r="B17" s="14"/>
+    </row>
+    <row r="18" ht="14.25">
+      <c r="B18" s="14"/>
+    </row>
+    <row r="19" ht="14.25">
+      <c r="B19" s="14"/>
+    </row>
+    <row r="20" ht="14.25">
+      <c r="B20" s="14"/>
+    </row>
+    <row r="21" ht="14.25">
+      <c r="B21" s="14"/>
+    </row>
+    <row r="22" ht="14.25">
+      <c r="B22" s="14"/>
+    </row>
+    <row r="23" ht="14.25">
+      <c r="B23" s="14"/>
+    </row>
+    <row r="24" ht="14.25">
+      <c r="B24" s="14"/>
+    </row>
+    <row r="25" ht="14.25">
+      <c r="B25" s="14"/>
+    </row>
+    <row r="26" ht="14.25">
+      <c r="B26" s="14"/>
+    </row>
+    <row r="27" ht="14.25">
+      <c r="B27" s="15"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="16"/>
+      <c r="I27" s="16"/>
+      <c r="J27" s="16"/>
+      <c r="K27" s="16"/>
+      <c r="L27" s="16"/>
+      <c r="M27" s="16"/>
+      <c r="N27" s="16"/>
+    </row>
+    <row r="28" ht="21">
+      <c r="B28" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C28" s="17"/>
+      <c r="F28" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="G28" s="18"/>
+      <c r="K28" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="L28" s="17"/>
+      <c r="M28" s="18"/>
+      <c r="N28" s="18"/>
+    </row>
+    <row r="31" ht="14.25"/>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="M28:N28"/>
+  </mergeCells>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup blackAndWhite="0" cellComments="none" copies="1" draft="0" errors="displayed" firstPageNumber="-1" fitToHeight="1" fitToWidth="1" horizontalDpi="600" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="0" usePrinterDefaults="1" verticalDpi="600"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>